<commit_message>
Ajout de l'enregistrement vocal
</commit_message>
<xml_diff>
--- a/Database/sub-03/beh/sub-03_task-work_questionnaire_beh.xlsx
+++ b/Database/sub-03/beh/sub-03_task-work_questionnaire_beh.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>647</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -530,16 +530,373 @@
           <t>--</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Utilisateur (Moi)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Code : Python, Java, Html </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Insignifiante</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>alt tab</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>687</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>alt tab</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>790</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Matériel</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Système (Machine)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Code : Python, Java, Html </t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Insignifiante</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>L'application freeze</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Matériel</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Système (Machine)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Code : Python, Java, Html </t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Insignifiante</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>l'application freeze</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3916</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>alt tab</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4020</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>alt tab</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4676</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Perturbation</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Utilisateur (Moi)</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Code : Python, Java, Html </t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Insignifiante</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Notification</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Faible</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>notification</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Plutôt fatigué</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Moyenne</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>run-01</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5003</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>alt tab</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Correction d'un problème avec stimulation du paramètre 3 dans Lua
</commit_message>
<xml_diff>
--- a/Database/sub-03/beh/sub-03_task-work_questionnaire_beh.xlsx
+++ b/Database/sub-03/beh/sub-03_task-work_questionnaire_beh.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>647</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -532,27 +532,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Prévention</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Utilisateur (Moi)</t>
+          <t>Système (Machine)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Code : Python, Java, Html </t>
+          <t xml:space="preserve">Bureautique : Word, Excel.. </t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Insignifiante</t>
+          <t>Assez Importante</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>alt tab</t>
+          <t>test</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -570,7 +570,7 @@
       <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -579,10 +579,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>687</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -593,11 +593,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>alt tab</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -605,7 +601,7 @@
       <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -614,7 +610,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>790</v>
+        <v>56</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -624,47 +620,19 @@
           <t>--</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Matériel</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Système (Machine)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Code : Python, Java, Html </t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Insignifiante</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>L'application freeze</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Neutre</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Neutre</t>
-        </is>
-      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -673,57 +641,27 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1150</v>
+        <v>66</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Matériel</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Système (Machine)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Code : Python, Java, Html </t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Insignifiante</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>l'application freeze</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Neutre</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Neutre</t>
-        </is>
-      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -732,7 +670,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3916</v>
+        <v>74</v>
       </c>
       <c r="D6" t="n">
         <v>3</v>
@@ -748,7 +686,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>alt tab</t>
+          <t>rapide</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -758,7 +696,7 @@
       <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -767,25 +705,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4020</v>
+        <v>85</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>alt tab</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -793,7 +725,7 @@
       <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,101 +734,42 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4676</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>--</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Perturbation</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Utilisateur (Moi)</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Code : Python, Java, Html </t>
+          <t>Test</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Insignifiante</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Notification</t>
-        </is>
-      </c>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Faible</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Oui</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>notification</t>
-        </is>
-      </c>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Plutôt fatigué</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Moyenne</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>run-01</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>5003</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>alt tab</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+          <t>Neutre</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>